<commit_message>
docs: Adding user id in comment api files
</commit_message>
<xml_diff>
--- a/api/Board/FreeComment_API.xlsx
+++ b/api/Board/FreeComment_API.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\AISW_Web_Community\api\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CC8FF8-1437-4B4F-A9A6-F44AF6F13DF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A43390-D1C8-4570-AA50-D1860C1B63C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="게시판 댓글 전체 조회" sheetId="1" r:id="rId1"/>
@@ -584,20 +584,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{
-   "transaction_time" : "2021-01-08T17:12:33.333",
-   "result_code" : "OK",
-   "description" : "OK",
-   "data" : {
-      "comment": "test",
-      "is_anonymous": "true",
-      "likes": 1,
-      "free_id": 1
-   }
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/board/free/comment/{id}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -977,6 +963,21 @@
       "is_anonymous": true,
       "likes": 1,
       "free_id": 1
+   }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+   "transaction_time" : "2021-01-08T17:12:33.333",
+   "result_code" : "OK",
+   "description" : "OK",
+   "data" : {
+      "comment": "test",
+      "is_anonymous": "true",
+      "likes": 1,
+      "free_id": 1,
+      "user_id": 1
    }
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1739,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B60143-E3B9-4AB4-9B51-6040CE152FCC}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:H34"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17"/>
@@ -2089,7 +2090,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
@@ -2113,7 +2114,7 @@
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -2124,7 +2125,7 @@
         <v>21</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2183,7 +2184,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="30"/>
       <c r="C28" s="30"/>
@@ -2195,11 +2196,11 @@
     </row>
     <row r="29" spans="1:8" ht="18.5" customHeight="1">
       <c r="A29" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="30"/>
@@ -2213,11 +2214,11 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="30"/>
       <c r="C30" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="30"/>
@@ -2231,11 +2232,11 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="30"/>
       <c r="C31" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D31" s="30"/>
       <c r="E31" s="30"/>
@@ -2249,11 +2250,11 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="30"/>
       <c r="C32" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -2264,7 +2265,7 @@
         <v>21</v>
       </c>
       <c r="H32" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2281,7 +2282,7 @@
     </row>
     <row r="34" spans="1:8" ht="354" customHeight="1">
       <c r="A34" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" s="36"/>
       <c r="C34" s="36"/>
@@ -2864,8 +2865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31E2576-20FD-4E47-B846-39903FF9702A}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:H35"/>
+    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17"/>
@@ -2881,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
@@ -3166,7 +3167,7 @@
     </row>
     <row r="19" spans="1:8" ht="177" customHeight="1">
       <c r="A19" s="35" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
@@ -3340,7 +3341,7 @@
     </row>
     <row r="29" spans="1:8" ht="19" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8" t="s">
@@ -3364,7 +3365,7 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="8"/>
@@ -3375,7 +3376,7 @@
         <v>21</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -3446,7 +3447,7 @@
     </row>
     <row r="35" spans="1:8" ht="221" customHeight="1">
       <c r="A35" s="56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="56"/>
       <c r="C35" s="56"/>
@@ -3892,6 +3893,7 @@
     <hyperlink ref="A18" r:id="rId2" xr:uid="{364A12D2-4995-4A23-A404-6A0D1A2185AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3916,7 +3918,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
@@ -3944,7 +3946,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
@@ -4065,7 +4067,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="61"/>
       <c r="C11" s="61"/>
@@ -4957,6 +4959,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="B14:H14"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
@@ -4966,13 +4975,6 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="B14:H14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
docs: Creating likes api files
</commit_message>
<xml_diff>
--- a/api/Board/FreeComment_API.xlsx
+++ b/api/Board/FreeComment_API.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\AISW_Web_Community\api\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E28EE5-F2C1-40E7-AF9E-8F39934947A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535A5FE6-2C3E-4C47-A5B6-5CE92D0DFBFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
   </bookViews>
   <sheets>
-    <sheet name="게시판 댓글 전체 조회" sheetId="1" r:id="rId1"/>
-    <sheet name="게시판 댓글 작성" sheetId="3" r:id="rId2"/>
-    <sheet name="게시판 댓글 삭제" sheetId="5" r:id="rId3"/>
+    <sheet name="게시판 댓글 좋아요" sheetId="6" r:id="rId1"/>
+    <sheet name="게시판 댓글 전체 조회" sheetId="1" r:id="rId2"/>
+    <sheet name="게시판 댓글 작성" sheetId="3" r:id="rId3"/>
+    <sheet name="게시판 댓글 삭제" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="100">
   <si>
     <t>Title</t>
   </si>
@@ -998,6 +999,82 @@
       "user_id": 1
    }
 }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>FreeComment (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>질문게시판</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>댓글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>좋아요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/free/comment/likes/{id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/board/free/comment/like/1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1269,7 +1346,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1353,6 +1430,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1397,51 +1484,51 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1452,9 +1539,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1769,6 +1860,840 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F87AE3-A69A-4ED1-A55A-0A7CCBF5F81A}">
+  <dimension ref="A1:H94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
+    <col min="2" max="7" width="13.25" style="1"/>
+    <col min="8" max="8" width="54.08203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="13.25" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A11" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="50"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="54"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="67"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" customHeight="1">
+      <c r="A19" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="36"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.5" customHeight="1">
+      <c r="A20" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.5" customHeight="1">
+      <c r="A26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.5" customHeight="1">
+      <c r="A27" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16" customHeight="1">
+      <c r="A28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="35"/>
+      <c r="C28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="19" customHeight="1">
+      <c r="A29" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="54"/>
+    </row>
+    <row r="30" spans="1:8" ht="224" customHeight="1">
+      <c r="A30" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+    </row>
+    <row r="35" ht="17" customHeight="1"/>
+    <row r="37" ht="225.5" customHeight="1"/>
+    <row r="45" ht="17" customHeight="1"/>
+    <row r="47" ht="17" customHeight="1"/>
+    <row r="49" spans="1:8" ht="18" customHeight="1"/>
+    <row r="51" spans="1:8" ht="18" customHeight="1"/>
+    <row r="54" spans="1:8" ht="318.5" customHeight="1"/>
+    <row r="62" spans="1:8">
+      <c r="A62" s="75"/>
+      <c r="B62" s="75"/>
+      <c r="C62" s="76"/>
+      <c r="D62" s="75"/>
+      <c r="E62" s="75"/>
+      <c r="F62" s="75"/>
+      <c r="G62" s="75"/>
+      <c r="H62" s="75"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="75"/>
+      <c r="B63" s="75"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="75"/>
+      <c r="F63" s="75"/>
+      <c r="G63" s="75"/>
+      <c r="H63" s="75"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="75"/>
+      <c r="B64" s="75"/>
+      <c r="C64" s="76"/>
+      <c r="D64" s="75"/>
+      <c r="E64" s="75"/>
+      <c r="F64" s="75"/>
+      <c r="G64" s="75"/>
+      <c r="H64" s="75"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="7"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="7"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="7"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="7"/>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="A6:H6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4F33C88E-2307-4CB6-A780-083AC067A138}"/>
+    <hyperlink ref="A12" r:id="rId2" xr:uid="{D24F2D39-D006-4E3E-BA8B-D19C287C223D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B60143-E3B9-4AB4-9B51-6040CE152FCC}">
   <dimension ref="A1:K94"/>
   <sheetViews>
@@ -1788,95 +2713,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
@@ -1925,64 +2850,64 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="46"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
@@ -2321,31 +3246,31 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="17" customHeight="1">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="50"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="54"/>
       <c r="K34" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="399.5" customHeight="1">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="41"/>
     </row>
     <row r="36" spans="1:11" ht="19" customHeight="1"/>
     <row r="37" spans="1:11" ht="19.5" customHeight="1"/>
@@ -2877,11 +3802,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31E2576-20FD-4E47-B846-39903FF9702A}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="A37" sqref="A37:H37"/>
     </sheetView>
   </sheetViews>
@@ -2897,95 +3822,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="55"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
@@ -3147,10 +4072,10 @@
       <c r="C16" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="70" t="s">
+      <c r="F16" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="70" t="s">
+      <c r="G16" s="38" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="23" t="s">
@@ -3178,66 +4103,66 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="59"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="57"/>
     </row>
     <row r="19" spans="1:8" ht="17" customHeight="1">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="62"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="64"/>
     </row>
     <row r="20" spans="1:8" ht="200.5" customHeight="1">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="41"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="54"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="65"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="67"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="28" t="s">
@@ -3490,28 +4415,28 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="17" customHeight="1">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="50"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="54"/>
     </row>
     <row r="37" spans="1:8" ht="271.5" customHeight="1">
-      <c r="A37" s="56" t="s">
+      <c r="A37" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
     </row>
     <row r="45" spans="1:8" ht="17" customHeight="1"/>
     <row r="47" spans="1:8" ht="17" customHeight="1"/>
@@ -3841,6 +4766,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="B22:H22"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B1:H1"/>
@@ -3849,12 +4780,6 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="B22:H22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3866,7 +4791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE8F0A6-CE1B-4868-9054-B38C338BA073}">
   <dimension ref="A1:H94"/>
   <sheetViews>
@@ -3886,95 +4811,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="55"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
@@ -4023,64 +4948,64 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="57"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="62"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="64"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="66"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="68"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="50"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="54"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="65"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="67"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="6" t="s">
@@ -4163,28 +5088,28 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
     </row>
     <row r="20" spans="1:8" ht="74" customHeight="1">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="41"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="12"/>
@@ -4307,24 +5232,24 @@
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="51"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
+      <c r="A33" s="68"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="52"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
     </row>
     <row r="35" spans="1:8" ht="19" customHeight="1">
       <c r="A35" s="16"/>
@@ -4928,6 +5853,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="B14:H14"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
@@ -4937,13 +5869,6 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="B14:H14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>